<commit_message>
OMC-130 Added code for add/edit/display address for the doctor profile
</commit_message>
<xml_diff>
--- a/SqlQueries/DataInsertUpdateQueries/Sprint 3/States.xlsx
+++ b/SqlQueries/DataInsertUpdateQueries/Sprint 3/States.xlsx
@@ -1103,8 +1103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D80"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D2" sqref="A1:D80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1137,7 +1137,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="str">
-        <f>CONCATENATE("INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (1,'",C2,"',1,1,GETDATE())")</f>
+        <f>CONCATENATE("INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (",B2,",'",C2,"',1,1,GETDATE())")</f>
         <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (1,'Andhra Pradesh',1,1,GETDATE())</v>
       </c>
     </row>
@@ -1152,7 +1152,7 @@
         <v>1</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3:D66" si="0">CONCATENATE("INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (1,'",C3,"',1,1,GETDATE())")</f>
+        <f t="shared" ref="D3:D66" si="0">CONCATENATE("INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (",B3,",'",C3,"',1,1,GETDATE())")</f>
         <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (1,'Arunachal Pradesh',1,1,GETDATE())</v>
       </c>
     </row>
@@ -1573,7 +1573,7 @@
       </c>
       <c r="D31" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (1,'Alabama',1,1,GETDATE())</v>
+        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (2,'Alabama',1,1,GETDATE())</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1588,7 +1588,7 @@
       </c>
       <c r="D32" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (1,'Alaska',1,1,GETDATE())</v>
+        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (2,'Alaska',1,1,GETDATE())</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1603,7 +1603,7 @@
       </c>
       <c r="D33" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (1,'Arizona',1,1,GETDATE())</v>
+        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (2,'Arizona',1,1,GETDATE())</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1618,7 +1618,7 @@
       </c>
       <c r="D34" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (1,'Arkansas',1,1,GETDATE())</v>
+        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (2,'Arkansas',1,1,GETDATE())</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1633,7 +1633,7 @@
       </c>
       <c r="D35" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (1,'California',1,1,GETDATE())</v>
+        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (2,'California',1,1,GETDATE())</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1648,7 +1648,7 @@
       </c>
       <c r="D36" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (1,'Colorado',1,1,GETDATE())</v>
+        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (2,'Colorado',1,1,GETDATE())</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1663,7 +1663,7 @@
       </c>
       <c r="D37" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (1,'Connecticut',1,1,GETDATE())</v>
+        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (2,'Connecticut',1,1,GETDATE())</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1678,7 +1678,7 @@
       </c>
       <c r="D38" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (1,'Delaware',1,1,GETDATE())</v>
+        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (2,'Delaware',1,1,GETDATE())</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1693,7 +1693,7 @@
       </c>
       <c r="D39" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (1,'Florida',1,1,GETDATE())</v>
+        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (2,'Florida',1,1,GETDATE())</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1708,7 +1708,7 @@
       </c>
       <c r="D40" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (1,'Georgia',1,1,GETDATE())</v>
+        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (2,'Georgia',1,1,GETDATE())</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1723,7 +1723,7 @@
       </c>
       <c r="D41" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (1,'Hawaii',1,1,GETDATE())</v>
+        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (2,'Hawaii',1,1,GETDATE())</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1738,7 +1738,7 @@
       </c>
       <c r="D42" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (1,'Idaho',1,1,GETDATE())</v>
+        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (2,'Idaho',1,1,GETDATE())</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1753,7 +1753,7 @@
       </c>
       <c r="D43" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (1,'Illinois',1,1,GETDATE())</v>
+        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (2,'Illinois',1,1,GETDATE())</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1768,7 +1768,7 @@
       </c>
       <c r="D44" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (1,'Indiana',1,1,GETDATE())</v>
+        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (2,'Indiana',1,1,GETDATE())</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1783,7 +1783,7 @@
       </c>
       <c r="D45" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (1,'Iowa',1,1,GETDATE())</v>
+        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (2,'Iowa',1,1,GETDATE())</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1798,7 +1798,7 @@
       </c>
       <c r="D46" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (1,'Kansas',1,1,GETDATE())</v>
+        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (2,'Kansas',1,1,GETDATE())</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1813,7 +1813,7 @@
       </c>
       <c r="D47" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (1,'Kentucky',1,1,GETDATE())</v>
+        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (2,'Kentucky',1,1,GETDATE())</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1828,7 +1828,7 @@
       </c>
       <c r="D48" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (1,'Louisiana',1,1,GETDATE())</v>
+        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (2,'Louisiana',1,1,GETDATE())</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -1843,7 +1843,7 @@
       </c>
       <c r="D49" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (1,'Maine',1,1,GETDATE())</v>
+        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (2,'Maine',1,1,GETDATE())</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -1858,7 +1858,7 @@
       </c>
       <c r="D50" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (1,'Maryland',1,1,GETDATE())</v>
+        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (2,'Maryland',1,1,GETDATE())</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -1873,7 +1873,7 @@
       </c>
       <c r="D51" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (1,'Massachusetts',1,1,GETDATE())</v>
+        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (2,'Massachusetts',1,1,GETDATE())</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -1888,7 +1888,7 @@
       </c>
       <c r="D52" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (1,'Michigan',1,1,GETDATE())</v>
+        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (2,'Michigan',1,1,GETDATE())</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -1903,7 +1903,7 @@
       </c>
       <c r="D53" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (1,'Minnesota',1,1,GETDATE())</v>
+        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (2,'Minnesota',1,1,GETDATE())</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -1918,7 +1918,7 @@
       </c>
       <c r="D54" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (1,'Mississippi',1,1,GETDATE())</v>
+        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (2,'Mississippi',1,1,GETDATE())</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -1933,7 +1933,7 @@
       </c>
       <c r="D55" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (1,'Missouri',1,1,GETDATE())</v>
+        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (2,'Missouri',1,1,GETDATE())</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -1948,7 +1948,7 @@
       </c>
       <c r="D56" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (1,'Montana',1,1,GETDATE())</v>
+        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (2,'Montana',1,1,GETDATE())</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -1963,7 +1963,7 @@
       </c>
       <c r="D57" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (1,'Nebraska',1,1,GETDATE())</v>
+        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (2,'Nebraska',1,1,GETDATE())</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -1978,7 +1978,7 @@
       </c>
       <c r="D58" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (1,'Nevada',1,1,GETDATE())</v>
+        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (2,'Nevada',1,1,GETDATE())</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -1993,7 +1993,7 @@
       </c>
       <c r="D59" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (1,'New Hampshire',1,1,GETDATE())</v>
+        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (2,'New Hampshire',1,1,GETDATE())</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -2008,7 +2008,7 @@
       </c>
       <c r="D60" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (1,'New Jersey',1,1,GETDATE())</v>
+        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (2,'New Jersey',1,1,GETDATE())</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -2023,7 +2023,7 @@
       </c>
       <c r="D61" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (1,'New Mexico',1,1,GETDATE())</v>
+        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (2,'New Mexico',1,1,GETDATE())</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -2038,7 +2038,7 @@
       </c>
       <c r="D62" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (1,'New York',1,1,GETDATE())</v>
+        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (2,'New York',1,1,GETDATE())</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -2053,7 +2053,7 @@
       </c>
       <c r="D63" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (1,'North Carolina',1,1,GETDATE())</v>
+        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (2,'North Carolina',1,1,GETDATE())</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -2068,7 +2068,7 @@
       </c>
       <c r="D64" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (1,'North Dakota',1,1,GETDATE())</v>
+        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (2,'North Dakota',1,1,GETDATE())</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -2083,7 +2083,7 @@
       </c>
       <c r="D65" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (1,'Ohio',1,1,GETDATE())</v>
+        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (2,'Ohio',1,1,GETDATE())</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -2098,7 +2098,7 @@
       </c>
       <c r="D66" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (1,'Oklahoma',1,1,GETDATE())</v>
+        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (2,'Oklahoma',1,1,GETDATE())</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -2112,8 +2112,8 @@
         <v>174</v>
       </c>
       <c r="D67" t="str">
-        <f t="shared" ref="D67:D80" si="1">CONCATENATE("INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (1,'",C67,"',1,1,GETDATE())")</f>
-        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (1,'Oregon',1,1,GETDATE())</v>
+        <f t="shared" ref="D67:D80" si="1">CONCATENATE("INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (",B67,",'",C67,"',1,1,GETDATE())")</f>
+        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (2,'Oregon',1,1,GETDATE())</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -2128,7 +2128,7 @@
       </c>
       <c r="D68" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (1,'Pennsylvania',1,1,GETDATE())</v>
+        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (2,'Pennsylvania',1,1,GETDATE())</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -2143,7 +2143,7 @@
       </c>
       <c r="D69" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (1,'Rhode Island',1,1,GETDATE())</v>
+        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (2,'Rhode Island',1,1,GETDATE())</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -2158,7 +2158,7 @@
       </c>
       <c r="D70" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (1,'South Carolina',1,1,GETDATE())</v>
+        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (2,'South Carolina',1,1,GETDATE())</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -2173,7 +2173,7 @@
       </c>
       <c r="D71" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (1,'South Dakota',1,1,GETDATE())</v>
+        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (2,'South Dakota',1,1,GETDATE())</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -2188,7 +2188,7 @@
       </c>
       <c r="D72" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (1,'Tennessee',1,1,GETDATE())</v>
+        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (2,'Tennessee',1,1,GETDATE())</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -2203,7 +2203,7 @@
       </c>
       <c r="D73" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (1,'Texas',1,1,GETDATE())</v>
+        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (2,'Texas',1,1,GETDATE())</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -2218,7 +2218,7 @@
       </c>
       <c r="D74" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (1,'Utah',1,1,GETDATE())</v>
+        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (2,'Utah',1,1,GETDATE())</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -2233,7 +2233,7 @@
       </c>
       <c r="D75" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (1,'Vermont',1,1,GETDATE())</v>
+        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (2,'Vermont',1,1,GETDATE())</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -2248,7 +2248,7 @@
       </c>
       <c r="D76" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (1,'Virginia',1,1,GETDATE())</v>
+        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (2,'Virginia',1,1,GETDATE())</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -2263,7 +2263,7 @@
       </c>
       <c r="D77" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (1,'Washington',1,1,GETDATE())</v>
+        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (2,'Washington',1,1,GETDATE())</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -2278,7 +2278,7 @@
       </c>
       <c r="D78" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (1,'West Virginia',1,1,GETDATE())</v>
+        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (2,'West Virginia',1,1,GETDATE())</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -2293,7 +2293,7 @@
       </c>
       <c r="D79" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (1,'Wisconsin',1,1,GETDATE())</v>
+        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (2,'Wisconsin',1,1,GETDATE())</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -2308,7 +2308,7 @@
       </c>
       <c r="D80" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (1,'Wyoming',1,1,GETDATE())</v>
+        <v>INSERT INTO [dbo].[StateMaster] ([CountryId] ,[State] ,[Active] ,[AddedBy] ,[AddedDate] ) VALUES   (2,'Wyoming',1,1,GETDATE())</v>
       </c>
     </row>
   </sheetData>
@@ -2331,7 +2331,7 @@
     <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="44.25" thickBot="1">
+    <row r="1" spans="1:5" ht="30.75" thickBot="1">
       <c r="A1" s="2">
         <v>1</v>
       </c>
@@ -2399,7 +2399,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="44.25" thickBot="1">
+    <row r="5" spans="1:5" ht="30.75" thickBot="1">
       <c r="A5" s="2">
         <v>5</v>
       </c>
@@ -2433,7 +2433,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="30.75" thickBot="1">
+    <row r="7" spans="1:5" ht="30" thickBot="1">
       <c r="A7" s="2">
         <v>7</v>
       </c>
@@ -2450,7 +2450,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="44.25" thickBot="1">
+    <row r="8" spans="1:5" ht="30" thickBot="1">
       <c r="A8" s="2">
         <v>8</v>
       </c>
@@ -2535,7 +2535,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="44.25" thickBot="1">
+    <row r="13" spans="1:5" ht="30.75" thickBot="1">
       <c r="A13" s="2">
         <v>13</v>
       </c>
@@ -2552,7 +2552,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="44.25" thickBot="1">
+    <row r="14" spans="1:5" ht="30.75" thickBot="1">
       <c r="A14" s="2">
         <v>14</v>
       </c>
@@ -2569,7 +2569,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="44.25" thickBot="1">
+    <row r="15" spans="1:5" ht="30.75" thickBot="1">
       <c r="A15" s="2">
         <v>15</v>
       </c>
@@ -2671,7 +2671,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="44.25" thickBot="1">
+    <row r="21" spans="1:5" ht="30" thickBot="1">
       <c r="A21" s="2">
         <v>21</v>
       </c>
@@ -2722,7 +2722,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="44.25" thickBot="1">
+    <row r="24" spans="1:5" ht="30" thickBot="1">
       <c r="A24" s="2">
         <v>24</v>
       </c>
@@ -2756,7 +2756,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="44.25" thickBot="1">
+    <row r="26" spans="1:5" ht="30" thickBot="1">
       <c r="A26" s="2">
         <v>26</v>
       </c>
@@ -2773,7 +2773,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="30.75" thickBot="1">
+    <row r="27" spans="1:5" ht="30" thickBot="1">
       <c r="A27" s="2">
         <v>27</v>
       </c>
@@ -2807,7 +2807,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="45.75" thickBot="1">
+    <row r="29" spans="1:5" ht="30" thickBot="1">
       <c r="A29" s="2">
         <v>29</v>
       </c>
@@ -2824,7 +2824,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="44.25" thickBot="1">
+    <row r="30" spans="1:5" ht="30" thickBot="1">
       <c r="A30" s="2">
         <v>30</v>
       </c>
@@ -2841,7 +2841,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="30.75" thickBot="1">
+    <row r="31" spans="1:5" ht="15.75" thickBot="1">
       <c r="A31" s="2">
         <v>31</v>
       </c>
@@ -2858,7 +2858,7 @@
         <v>4389</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="30.75" thickBot="1">
+    <row r="32" spans="1:5" ht="30" thickBot="1">
       <c r="A32" s="2">
         <v>32</v>
       </c>
@@ -2875,7 +2875,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="44.25" thickBot="1">
+    <row r="33" spans="1:5" ht="30" thickBot="1">
       <c r="A33" s="2">
         <v>33</v>
       </c>
@@ -2892,7 +2892,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="44.25" thickBot="1">
+    <row r="34" spans="1:5" ht="30" thickBot="1">
       <c r="A34" s="2">
         <v>34</v>
       </c>
@@ -2943,7 +2943,7 @@
         <v>2877</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="44.25" thickBot="1">
+    <row r="37" spans="1:5" ht="30" thickBot="1">
       <c r="A37" s="2">
         <v>37</v>
       </c>
@@ -2960,7 +2960,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="44.25" thickBot="1">
+    <row r="38" spans="1:5" ht="30.75" thickBot="1">
       <c r="A38" s="2">
         <v>38</v>
       </c>
@@ -3011,7 +3011,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="44.25" thickBot="1">
+    <row r="41" spans="1:5" ht="30" thickBot="1">
       <c r="A41" s="2">
         <v>41</v>
       </c>
@@ -3045,7 +3045,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="44.25" thickBot="1">
+    <row r="43" spans="1:5" ht="30" thickBot="1">
       <c r="A43" s="2">
         <v>43</v>
       </c>
@@ -3113,7 +3113,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="44.25" thickBot="1">
+    <row r="47" spans="1:5" ht="30" thickBot="1">
       <c r="A47" s="2">
         <v>47</v>
       </c>
@@ -3147,7 +3147,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="30.75" thickBot="1">
+    <row r="49" spans="1:5" ht="30" thickBot="1">
       <c r="A49" s="2">
         <v>49</v>
       </c>

</xml_diff>